<commit_message>
oct 1 stuff - spreadsheet column name changes
</commit_message>
<xml_diff>
--- a/backend/api/app_templates/forecast_report_template.xlsx
+++ b/backend/api/app_templates/forecast_report_template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A169DD8-1255-E247-B931-974A4A5B1827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D33629-2BBF-3F42-A22D-B60FA09C2465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2460" windowWidth="27640" windowHeight="16940" xr2:uid="{3E367DA1-2811-4C43-8C2A-70EAFD4D2A2F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{3E367DA1-2811-4C43-8C2A-70EAFD4D2A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Forecast Report" sheetId="2" r:id="rId2"/>
+    <sheet name="Dropdowns" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029" calcOnSave="0"/>
   <extLst>
@@ -37,47 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Please note that:</t>
   </si>
   <si>
-    <t>(2) "make" should be no more than 250 characters</t>
-  </si>
-  <si>
-    <t>(4) "type" should be exactly one of: BEV, PHEV, FCEV, EREV</t>
-  </si>
-  <si>
-    <t>(5) "range" should be a real number with no more than 2 decimal places</t>
-  </si>
-  <si>
-    <t>make</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>modelYear</t>
-  </si>
-  <si>
-    <t>modelName</t>
-  </si>
-  <si>
-    <t>zevClass</t>
-  </si>
-  <si>
-    <t>(3) "modelName" should be no more than 250 characters</t>
-  </si>
-  <si>
-    <t>(6) "zevClass" should be a single, uppercase letter</t>
-  </si>
-  <si>
-    <t>(1) "modelYear" should be a 4 digit integer</t>
-  </si>
-  <si>
     <t>Please fill out the "Forecast Report" sheet</t>
   </si>
   <si>
@@ -87,27 +52,143 @@
     <t>Please do not alter any of the header names in the "Forecast Report" sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">Please note that all of the fields in the "Forecast Report" sheet are mandatory </t>
-  </si>
-  <si>
-    <t>(8) "totalSupplied" should be an integer</t>
-  </si>
-  <si>
-    <t>totalSupplied</t>
-  </si>
-  <si>
-    <t>vehicleClass</t>
-  </si>
-  <si>
-    <t>(7) "vehicleClass" should be no more than 250 characters</t>
+    <t>Model Year</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>ZEV Class</t>
+  </si>
+  <si>
+    <t>Vehicle Class and Interior Volume</t>
+  </si>
+  <si>
+    <t>Total ZEVs Supplied</t>
+  </si>
+  <si>
+    <t>BEV</t>
+  </si>
+  <si>
+    <t>PHEV</t>
+  </si>
+  <si>
+    <t>EREV</t>
+  </si>
+  <si>
+    <t>FCEV</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Two-seater</t>
+  </si>
+  <si>
+    <t>Minicompact (less than 85 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Subcompact (85–99 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Compact (100–109 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Mid-size (110–119 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Full-size (120 cu. ft. or more)</t>
+  </si>
+  <si>
+    <t>Station wagon: Mid-size (130–159 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Station wagon: Small (less than 130 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Pickup truck: Small (less than 2,722 kg)</t>
+  </si>
+  <si>
+    <t>Pickup truck: Standard (2,722–3,856 kg)</t>
+  </si>
+  <si>
+    <t>Sport utility vehicle: Small (less than 2,722 kg)</t>
+  </si>
+  <si>
+    <t>Sport utility vehicle: Standard (2,722–4,536 kg)</t>
+  </si>
+  <si>
+    <t>Minivan (less than 3,856 kg)</t>
+  </si>
+  <si>
+    <t>Van: Cargo (less than 3,856 kg)</t>
+  </si>
+  <si>
+    <t>Van: Passenger (less than 4,536 kg)</t>
+  </si>
+  <si>
+    <t>Special purpose vehicle (less than 3,856 kg)</t>
+  </si>
+  <si>
+    <t>(1) "Model Year" should be a 4 digit integer</t>
+  </si>
+  <si>
+    <t>(2) "Make" should be no more than 250 characters</t>
+  </si>
+  <si>
+    <t>(3) "Model" should be no more than 250 characters</t>
+  </si>
+  <si>
+    <t>(4) "Type" should be exactly one of: BEV, PHEV, FCEV, EREV</t>
+  </si>
+  <si>
+    <t>(5) "Range" should be a real number with no more than 2 decimal places</t>
+  </si>
+  <si>
+    <t>(6) "ZEV Class" should be a single, uppercase letter</t>
+  </si>
+  <si>
+    <t>(7) "Vehicle Class and Interior Volume" should be no more than 250 characters</t>
+  </si>
+  <si>
+    <t>(8) "Total ZEVs Supplied" should be an integer</t>
+  </si>
+  <si>
+    <t>Other/TBD</t>
+  </si>
+  <si>
+    <t>Please note that no field in the "Forecast Report" sheet may be blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -135,8 +216,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,29 +557,29 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -507,42 +589,42 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -555,41 +637,201 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABA7BD-FA5A-AB47-AC69-5AFF4A29011C}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39AFB65F-9925-4948-9A48-C7B4DCB7305D}">
+          <x14:formula1>
+            <xm:f>Dropdowns!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D200</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D6D3C224-EFF6-4699-A663-BC2AB9770A59}">
+          <x14:formula1>
+            <xm:f>Dropdowns!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F200</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{772A5E7C-AB2C-4F52-B38D-0B665D05240D}">
+          <x14:formula1>
+            <xm:f>Dropdowns!$C$2:$C$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G200</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E032F77C-386B-40FF-9326-AA2E46F58A00}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oct 1 stuff - spreadsheet column name changes (#2225)
</commit_message>
<xml_diff>
--- a/backend/api/app_templates/forecast_report_template.xlsx
+++ b/backend/api/app_templates/forecast_report_template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A169DD8-1255-E247-B931-974A4A5B1827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D33629-2BBF-3F42-A22D-B60FA09C2465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2460" windowWidth="27640" windowHeight="16940" xr2:uid="{3E367DA1-2811-4C43-8C2A-70EAFD4D2A2F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{3E367DA1-2811-4C43-8C2A-70EAFD4D2A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Forecast Report" sheetId="2" r:id="rId2"/>
+    <sheet name="Dropdowns" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029" calcOnSave="0"/>
   <extLst>
@@ -37,47 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Please note that:</t>
   </si>
   <si>
-    <t>(2) "make" should be no more than 250 characters</t>
-  </si>
-  <si>
-    <t>(4) "type" should be exactly one of: BEV, PHEV, FCEV, EREV</t>
-  </si>
-  <si>
-    <t>(5) "range" should be a real number with no more than 2 decimal places</t>
-  </si>
-  <si>
-    <t>make</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>modelYear</t>
-  </si>
-  <si>
-    <t>modelName</t>
-  </si>
-  <si>
-    <t>zevClass</t>
-  </si>
-  <si>
-    <t>(3) "modelName" should be no more than 250 characters</t>
-  </si>
-  <si>
-    <t>(6) "zevClass" should be a single, uppercase letter</t>
-  </si>
-  <si>
-    <t>(1) "modelYear" should be a 4 digit integer</t>
-  </si>
-  <si>
     <t>Please fill out the "Forecast Report" sheet</t>
   </si>
   <si>
@@ -87,27 +52,143 @@
     <t>Please do not alter any of the header names in the "Forecast Report" sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">Please note that all of the fields in the "Forecast Report" sheet are mandatory </t>
-  </si>
-  <si>
-    <t>(8) "totalSupplied" should be an integer</t>
-  </si>
-  <si>
-    <t>totalSupplied</t>
-  </si>
-  <si>
-    <t>vehicleClass</t>
-  </si>
-  <si>
-    <t>(7) "vehicleClass" should be no more than 250 characters</t>
+    <t>Model Year</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>ZEV Class</t>
+  </si>
+  <si>
+    <t>Vehicle Class and Interior Volume</t>
+  </si>
+  <si>
+    <t>Total ZEVs Supplied</t>
+  </si>
+  <si>
+    <t>BEV</t>
+  </si>
+  <si>
+    <t>PHEV</t>
+  </si>
+  <si>
+    <t>EREV</t>
+  </si>
+  <si>
+    <t>FCEV</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Two-seater</t>
+  </si>
+  <si>
+    <t>Minicompact (less than 85 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Subcompact (85–99 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Compact (100–109 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Mid-size (110–119 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Full-size (120 cu. ft. or more)</t>
+  </si>
+  <si>
+    <t>Station wagon: Mid-size (130–159 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Station wagon: Small (less than 130 cu. ft.)</t>
+  </si>
+  <si>
+    <t>Pickup truck: Small (less than 2,722 kg)</t>
+  </si>
+  <si>
+    <t>Pickup truck: Standard (2,722–3,856 kg)</t>
+  </si>
+  <si>
+    <t>Sport utility vehicle: Small (less than 2,722 kg)</t>
+  </si>
+  <si>
+    <t>Sport utility vehicle: Standard (2,722–4,536 kg)</t>
+  </si>
+  <si>
+    <t>Minivan (less than 3,856 kg)</t>
+  </si>
+  <si>
+    <t>Van: Cargo (less than 3,856 kg)</t>
+  </si>
+  <si>
+    <t>Van: Passenger (less than 4,536 kg)</t>
+  </si>
+  <si>
+    <t>Special purpose vehicle (less than 3,856 kg)</t>
+  </si>
+  <si>
+    <t>(1) "Model Year" should be a 4 digit integer</t>
+  </si>
+  <si>
+    <t>(2) "Make" should be no more than 250 characters</t>
+  </si>
+  <si>
+    <t>(3) "Model" should be no more than 250 characters</t>
+  </si>
+  <si>
+    <t>(4) "Type" should be exactly one of: BEV, PHEV, FCEV, EREV</t>
+  </si>
+  <si>
+    <t>(5) "Range" should be a real number with no more than 2 decimal places</t>
+  </si>
+  <si>
+    <t>(6) "ZEV Class" should be a single, uppercase letter</t>
+  </si>
+  <si>
+    <t>(7) "Vehicle Class and Interior Volume" should be no more than 250 characters</t>
+  </si>
+  <si>
+    <t>(8) "Total ZEVs Supplied" should be an integer</t>
+  </si>
+  <si>
+    <t>Other/TBD</t>
+  </si>
+  <si>
+    <t>Please note that no field in the "Forecast Report" sheet may be blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -135,8 +216,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,29 +557,29 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -507,42 +589,42 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -555,41 +637,201 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABA7BD-FA5A-AB47-AC69-5AFF4A29011C}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39AFB65F-9925-4948-9A48-C7B4DCB7305D}">
+          <x14:formula1>
+            <xm:f>Dropdowns!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D200</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D6D3C224-EFF6-4699-A663-BC2AB9770A59}">
+          <x14:formula1>
+            <xm:f>Dropdowns!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F200</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{772A5E7C-AB2C-4F52-B38D-0B665D05240D}">
+          <x14:formula1>
+            <xm:f>Dropdowns!$C$2:$C$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G200</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E032F77C-386B-40FF-9326-AA2E46F58A00}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 2219 - forecast report colum mapping + automatic summation of ZEVs supplied
</commit_message>
<xml_diff>
--- a/backend/api/app_templates/forecast_report_template.xlsx
+++ b/backend/api/app_templates/forecast_report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D33629-2BBF-3F42-A22D-B60FA09C2465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FD8B1-2FDC-CE49-B9CB-38CA0E15DAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{3E367DA1-2811-4C43-8C2A-70EAFD4D2A2F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Please note that:</t>
   </si>
@@ -64,18 +64,12 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
     <t>ZEV Class</t>
   </si>
   <si>
     <t>Vehicle Class and Interior Volume</t>
   </si>
   <si>
-    <t>Total ZEVs Supplied</t>
-  </si>
-  <si>
     <t>BEV</t>
   </si>
   <si>
@@ -166,13 +160,25 @@
     <t>(7) "Vehicle Class and Interior Volume" should be no more than 250 characters</t>
   </si>
   <si>
-    <t>(8) "Total ZEVs Supplied" should be an integer</t>
-  </si>
-  <si>
     <t>Other/TBD</t>
   </si>
   <si>
     <t>Please note that no field in the "Forecast Report" sheet may be blank</t>
+  </si>
+  <si>
+    <t>ZEVs Supply Forecast</t>
+  </si>
+  <si>
+    <t>(8) "ZEVs Supply Forecast" should be an integer</t>
+  </si>
+  <si>
+    <t>Please note that there must be at least one record in the "Forecast Report" sheet</t>
+  </si>
+  <si>
+    <t>Please note that there must be no more than 2000 records in the "Forecast Report" sheet</t>
+  </si>
+  <si>
+    <t>Range (km)</t>
   </si>
 </sst>
 </file>
@@ -553,13 +559,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3882FB2-E1FB-7145-985F-5D4D3D2256D4}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" customWidth="1"/>
+    <col min="1" max="1" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -584,47 +590,57 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +661,7 @@
   <cols>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -662,16 +678,16 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -722,116 +738,116 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 2219 - forecast report column mapping + automatic summation of ZEVs supplied (#2231)
* feat: 2219 - forecast report colum mapping + automatic summation of ZEVs supplied

* small change

* fix totals display upon discard of records
</commit_message>
<xml_diff>
--- a/backend/api/app_templates/forecast_report_template.xlsx
+++ b/backend/api/app_templates/forecast_report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D33629-2BBF-3F42-A22D-B60FA09C2465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FD8B1-2FDC-CE49-B9CB-38CA0E15DAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{3E367DA1-2811-4C43-8C2A-70EAFD4D2A2F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Please note that:</t>
   </si>
@@ -64,18 +64,12 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
     <t>ZEV Class</t>
   </si>
   <si>
     <t>Vehicle Class and Interior Volume</t>
   </si>
   <si>
-    <t>Total ZEVs Supplied</t>
-  </si>
-  <si>
     <t>BEV</t>
   </si>
   <si>
@@ -166,13 +160,25 @@
     <t>(7) "Vehicle Class and Interior Volume" should be no more than 250 characters</t>
   </si>
   <si>
-    <t>(8) "Total ZEVs Supplied" should be an integer</t>
-  </si>
-  <si>
     <t>Other/TBD</t>
   </si>
   <si>
     <t>Please note that no field in the "Forecast Report" sheet may be blank</t>
+  </si>
+  <si>
+    <t>ZEVs Supply Forecast</t>
+  </si>
+  <si>
+    <t>(8) "ZEVs Supply Forecast" should be an integer</t>
+  </si>
+  <si>
+    <t>Please note that there must be at least one record in the "Forecast Report" sheet</t>
+  </si>
+  <si>
+    <t>Please note that there must be no more than 2000 records in the "Forecast Report" sheet</t>
+  </si>
+  <si>
+    <t>Range (km)</t>
   </si>
 </sst>
 </file>
@@ -553,13 +559,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3882FB2-E1FB-7145-985F-5D4D3D2256D4}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" customWidth="1"/>
+    <col min="1" max="1" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -584,47 +590,57 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +661,7 @@
   <cols>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -662,16 +678,16 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -722,116 +738,116 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>